<commit_message>
Added details to README file
</commit_message>
<xml_diff>
--- a/data/data_test.xlsx
+++ b/data/data_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\Automation Testing\Selenium\PegaF&amp;D\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3504B1A-D0C4-4E7A-9BDB-5E9CA7A44A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F7C78-42CD-4345-87FA-48DFDE326758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7560" yWindow="0" windowWidth="10340" windowHeight="10080" xr2:uid="{2B756A7A-3F63-4D06-99EF-F38828F3BCE4}"/>
   </bookViews>
@@ -448,9 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17286D6D-1B54-4A8F-8E39-47B6C0A5D3C9}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>